<commit_message>
Llenado de plantilla de primera iteración
Se agregaron los tiempos tomados en las tareas correspondientes a cada integrante
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26480" windowHeight="14020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26475" windowHeight="14025"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
     <sheet name="Instructivo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Columna</t>
   </si>
@@ -45,17 +50,6 @@
   </si>
   <si>
     <t>Identificador (ID) de CU</t>
-  </si>
-  <si>
-    <t>CU-XX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La [clase de usuario o actor] deberá poder [hacer algo] [para algún objeto] [condiciones, tiempo de respuesta o declaración de calidad].
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La [clase de usuario o actor] deberá poder [hacer algo] [para algún objeto] [condiciones, tiempo de respuesta o declaración de calidad]
-</t>
   </si>
   <si>
     <t>Código que identifica al Caso de Uso de forma unívoca, una vez asignado, no debe ser re-usado en otro Caso de Uso, ni siquiera si el CU es descartado. El código identifica el CU otros documentos, como por ejemplo la plantilla de descripción de CU.</t>
@@ -113,12 +107,196 @@
   <si>
     <t xml:space="preserve">El incremento en el que se incluye el Caso de Uso. Esta asignación puede cambiar en cada iteración donde se haga la revisión del producto, según las prioridades indicadas por el dueño del producto. </t>
   </si>
+  <si>
+    <t>CU-01</t>
+  </si>
+  <si>
+    <t>Administrar alumno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El director debe poder registrar a los alumnos en el sistema, con el fin de que los maestros puedan añadirlos a sus respectivos grupos. Además, de poder editar información personal del alumno para mantener su información actualizada.
+</t>
+  </si>
+  <si>
+    <t>CU-02</t>
+  </si>
+  <si>
+    <t>Administrar profesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>CU-03</t>
+  </si>
+  <si>
+    <t>Administrar grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El director debe poder crear y eliminar grupos, para que mediante ellos el maestro pueda llevar un control de sus horarios, alumnos e inscripciones.
+</t>
+  </si>
+  <si>
+    <t>Rentar espacio</t>
+  </si>
+  <si>
+    <t>CU-04</t>
+  </si>
+  <si>
+    <t>CU-05</t>
+  </si>
+  <si>
+    <t>Definir horario</t>
+  </si>
+  <si>
+    <t>CU-06</t>
+  </si>
+  <si>
+    <t>Registrar pago colaborador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El director debe poder registrar los pagos de los maestros, para llevar un control de las fechas de pago, así como de los ingresos obtenidos.
+</t>
+  </si>
+  <si>
+    <t>CU-07</t>
+  </si>
+  <si>
+    <t>Consultar ingresos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El director debe poder llevar registro de todos los ingresos obtenidos, para llevar un control tanto de los pagos de los colaboradores, como de las rentas realizadas.
+</t>
+  </si>
+  <si>
+    <t>CU-08</t>
+  </si>
+  <si>
+    <t>Registrar pago alumno</t>
+  </si>
+  <si>
+    <t>CU-09</t>
+  </si>
+  <si>
+    <t>Consultar recibos de alumnos</t>
+  </si>
+  <si>
+    <t>CU-10</t>
+  </si>
+  <si>
+    <t>Consultar notificaciones director</t>
+  </si>
+  <si>
+    <t>CU-11</t>
+  </si>
+  <si>
+    <t>Registrar campaña publicitaria</t>
+  </si>
+  <si>
+    <t>CU-12</t>
+  </si>
+  <si>
+    <t>Administrar egresos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El director debe poder llevar un registro de todos los gastos realizados para tener un control de estos.
+</t>
+  </si>
+  <si>
+    <t>CU-13</t>
+  </si>
+  <si>
+    <t>Consultar estadísticas</t>
+  </si>
+  <si>
+    <t>El director debe poder visualizar las estadísticas, con el fin de analizar los datos de ingresos y egresos de una manera gráfica.</t>
+  </si>
+  <si>
+    <t>CU-14</t>
+  </si>
+  <si>
+    <t>Administar Inscripciones</t>
+  </si>
+  <si>
+    <t>El maestro debe poder inscribir, reinscribir o dar de baja alumnos en los grupos correspondientes, para llevar un control tanto de los alumnos como de los pagos de inscripción y reinscripción.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+El director debe poder ver los próximos pagos que sus colaboradores deberán realizar, así como de los días que se llevarán a cabo las rentas programadas, con el fin de mantenerse informado.</t>
+  </si>
+  <si>
+    <t>CU-15</t>
+  </si>
+  <si>
+    <t>Administrar asistencia de alumnos</t>
+  </si>
+  <si>
+    <t>El maestro debe poder verificar la asistencia de sus alumnos a las clases, para llevar un control de los días que asisten los estudiantes con respecto a los pagos realizados.</t>
+  </si>
+  <si>
+    <t>CU-16</t>
+  </si>
+  <si>
+    <t>Cobrar mensualidad</t>
+  </si>
+  <si>
+    <t>CU-17</t>
+  </si>
+  <si>
+    <t>Visualizar historial de pagos</t>
+  </si>
+  <si>
+    <t>El maestro debe poder ver todos los pagos que sus alumnos han realizado, con el fin de tener un mejor control de sus pagos.</t>
+  </si>
+  <si>
+    <t>CU-18</t>
+  </si>
+  <si>
+    <t>Administrar promoción</t>
+  </si>
+  <si>
+    <t>El maestro debe poder crear promociones, con el fin de aplicarlas en los pagos mensuales o inscripciones de los alumnos.</t>
+  </si>
+  <si>
+    <t>CU-19</t>
+  </si>
+  <si>
+    <t>Consultar grupos</t>
+  </si>
+  <si>
+    <t>El maestro debe poder visualizar sus grupos, con el fin de tener un mejor control sus alumnos.</t>
+  </si>
+  <si>
+    <t>CU-20</t>
+  </si>
+  <si>
+    <t>CU-21</t>
+  </si>
+  <si>
+    <t>Consultar notificaciones maestro</t>
+  </si>
+  <si>
+    <t>El maestro debe poder ver los próximos pagos que sus alumnos deberán realizar, con el fin de mantenerse informado de los días que recibirá los pagos correspondientes a la mensualidad.</t>
+  </si>
+  <si>
+    <t>El director debe poder registrar clientes en el sistema, con el fin de tener un mejor control de sus pagos de renta, así como poder editar información personal del cliente para mantener su información actualizada.</t>
+  </si>
+  <si>
+    <t>Administrar cliente</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +339,19 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,7 +408,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -233,6 +424,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -243,6 +446,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -531,43 +742,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="49" style="2" customWidth="1"/>
-    <col min="10" max="10" width="39.33203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="39.28515625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="36">
+    <row r="1" spans="2:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" ht="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -576,10 +787,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>3</v>
@@ -588,204 +799,471 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="42">
+    <row r="5" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="12">
+        <v>18</v>
+      </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="42">
+    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="12">
+        <v>18</v>
+      </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:9" ht="42">
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="12">
+        <v>18</v>
+      </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="2:9" ht="42">
+    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="12">
+        <v>16</v>
+      </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:9" ht="42">
+    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="12">
+        <v>18</v>
+      </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:9" ht="42">
+    <row r="10" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="12">
+        <v>14</v>
+      </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" ht="42">
+    <row r="11" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="12">
+        <v>16</v>
+      </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="2:9" ht="42">
+    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="12">
+        <v>14</v>
+      </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:9" ht="42">
+    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="12">
+        <v>14</v>
+      </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="2:9" ht="42">
-      <c r="B14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+    <row r="14" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="12">
+        <v>14</v>
+      </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:9" ht="42">
+    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="12">
+        <v>16</v>
+      </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="2:9" ht="42">
+    <row r="16" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="12">
+        <v>18</v>
+      </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:9" ht="42">
+    <row r="17" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="12">
+        <v>12</v>
+      </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="42">
+    <row r="18" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="12">
+        <v>20</v>
+      </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="12">
+        <v>16</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="12">
+        <v>14</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="12">
+        <v>14</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="12">
+        <v>16</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="12">
+        <v>14</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="12">
+        <v>14</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="12">
+        <v>18</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -798,30 +1276,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B8" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B8" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="86" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="2.85546875" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="36">
+    <row r="1" spans="2:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,72 +1307,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="42">
+    <row r="5" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="168">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="210" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="24" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Plantilla de casos de uso completada
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Documentos\Repositorios\DesarrolloSW\ProyectoDesarrolloSW-EQ1\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26475" windowHeight="14025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
   <si>
     <t>Columna</t>
   </si>
@@ -124,10 +124,6 @@
     <t>Administrar profesor</t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t>CU-03</t>
   </si>
   <si>
@@ -290,12 +286,33 @@
   </si>
   <si>
     <t>Alta</t>
+  </si>
+  <si>
+    <t>El director debe poder  asignar lapsos a una actividad a ser realizada, con el fin de evitar traslapes y conocer en todo momento la disponibilidad de los espacios</t>
+  </si>
+  <si>
+    <t>El director debe poder  visualizar, registrar y editar los datos de rentas de aulas, con el fin de llevar un control de los espacios y su disponibilidad</t>
+  </si>
+  <si>
+    <t>El director debe poder manipular la información de los colaboradores en el sistema, para así poder relacionar pagos, asignar grupos y horarios de las actividades respectivas a cada colaborador</t>
+  </si>
+  <si>
+    <t>El director debe poder almacenar los pagos recibidos por parte de los alumnos para sus colaboradores para ampliar la disponibilidad de los cobros</t>
+  </si>
+  <si>
+    <t>El director debe poder visualizar los detalles de los pagos que ha recibido por parte de los alumnos para saber con certeza los movimientos pendientes de realizar</t>
+  </si>
+  <si>
+    <t>El director debe poder almacenar los datos de las campañas publicitarias que se han creado, con el fin de tener actualizados en todo momento la duración, campañas activas y egresos relacionados a las campañas</t>
+  </si>
+  <si>
+    <t>El maestro debe poder registrar los pagos realizados por los alumnos, para llevar un control de ingresos y pagos pendientes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,8 +461,36 @@
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{6816A1C2-B94E-42CF-BE4B-EE9A1207F6A2}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -741,11 +786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,454 +855,454 @@
         <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="12">
         <v>18</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="12">
         <v>18</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="12">
         <v>18</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="12">
         <v>16</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="12">
         <v>18</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="12">
         <v>14</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="12">
         <v>16</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="12">
         <v>14</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="12">
         <v>14</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="12">
         <v>14</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="12">
         <v>16</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="12">
         <v>18</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="12">
         <v>12</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="12">
         <v>20</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" s="12">
         <v>16</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="12">
         <v>14</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" s="12">
         <v>14</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" s="12">
         <v>16</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="12">
         <v>14</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="12">
         <v>14</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="12">
         <v>18</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I25" s="6"/>
     </row>
@@ -1273,7 +1318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="B8" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>